<commit_message>
chore: remove dataset_description.json and README files for auto_events; update create_events_tsv.py to centralize video duration loading and improve event filtering while preserving original order; enhance detect_markers.py with new command line options for saving annotations
</commit_message>
<xml_diff>
--- a/data/sourcedata/xdf/sub-12/order_matrix_12_A_block1_VR.xlsx
+++ b/data/sourcedata/xdf/sub-12/order_matrix_12_A_block1_VR.xlsx
@@ -498,7 +498,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -517,7 +517,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>./instructions_videos/2_baseline_instructions_text.mp4</t>
+          <t>./instructions_videos/VR/2_baseline_instructions_text.mp4</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -536,7 +536,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -574,7 +574,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -593,7 +593,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>./instructions_videos/initial_relaxation_video_text.mp4</t>
+          <t>./instructions_videos/VR/initial_relaxation_video_text.mp4</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -612,7 +612,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -650,7 +650,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -669,7 +669,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_1_text.mp4</t>
+          <t>./instructions_videos/VR/block_1_text.mp4</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -690,7 +690,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -723,7 +723,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/9.mp4</t>
+          <t>../stimuli/exp_videos/VR/8.mp4</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -744,7 +744,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -763,7 +763,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+          <t>./instructions_videos/VR/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -784,7 +784,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -824,7 +824,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -843,7 +843,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>./instructions_videos/VR/confidence_verbal_report_text.mp4</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -864,7 +864,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -883,7 +883,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>./instructions_videos/mareo.mp4</t>
+          <t>./instructions_videos/VR/mareo.mp4</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -904,7 +904,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -923,7 +923,7 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_1_text_reminder.mp4</t>
+          <t>./instructions_videos/VR/block_1_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -944,7 +944,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -962,7 +962,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -977,7 +977,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/8.mp4</t>
+          <t>../stimuli/exp_videos/VR/9.mp4</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -998,7 +998,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1017,7 +1017,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+          <t>./instructions_videos/VR/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1038,7 +1038,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1078,7 +1078,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>./instructions_videos/VR/confidence_verbal_report_text.mp4</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1118,7 +1118,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1137,7 +1137,7 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>./instructions_videos/mareo.mp4</t>
+          <t>./instructions_videos/VR/mareo.mp4</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1158,7 +1158,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1177,7 +1177,7 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_1_text_reminder.mp4</t>
+          <t>./instructions_videos/VR/block_1_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1198,7 +1198,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1216,7 +1216,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/7.mp4</t>
+          <t>../stimuli/exp_videos/VR/4.mp4</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1252,7 +1252,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1271,7 +1271,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+          <t>./instructions_videos/VR/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1292,7 +1292,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1332,7 +1332,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1351,7 +1351,7 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>./instructions_videos/VR/confidence_verbal_report_text.mp4</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1372,7 +1372,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1391,7 +1391,7 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>./instructions_videos/mareo.mp4</t>
+          <t>./instructions_videos/VR/mareo.mp4</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -1412,7 +1412,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1431,7 +1431,7 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>./instructions_videos/block_1_text_reminder.mp4</t>
+          <t>./instructions_videos/VR/block_1_text_reminder.mp4</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -1452,7 +1452,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>../stimuli/exp_videos/VR/4.mp4</t>
+          <t>../stimuli/exp_videos/VR/7.mp4</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -1506,7 +1506,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1525,7 +1525,7 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>./instructions_videos/post_stimulus_verbal_report.mp4</t>
+          <t>./instructions_videos/VR/post_stimulus_verbal_report.mp4</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -1546,7 +1546,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1586,7 +1586,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1605,7 +1605,7 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_verbal_report_text.mp4</t>
+          <t>./instructions_videos/VR/confidence_verbal_report_text.mp4</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -1626,7 +1626,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1645,7 +1645,7 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>./instructions_videos/mareo.mp4</t>
+          <t>./instructions_videos/VR/mareo.mp4</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -1666,7 +1666,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1685,7 +1685,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>./instructions_videos/luminance_instructions_direct.mp4</t>
+          <t>./instructions_videos/VR/luminance_instructions_direct.mp4</t>
         </is>
       </c>
       <c r="I30" t="inlineStr"/>
@@ -1704,7 +1704,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1752,7 +1752,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1771,7 +1771,7 @@
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>./instructions_videos/confidence_luminance_practice_instructions_text.mp4</t>
+          <t>./instructions_videos/VR/confidence_luminance_practice_instructions_text.mp4</t>
         </is>
       </c>
       <c r="I32" t="inlineStr"/>
@@ -1790,7 +1790,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1809,7 +1809,7 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>./instructions_videos/rest_suprablock_text.mp4</t>
+          <t>./instructions_videos/VR/rest_suprablock_text.mp4</t>
         </is>
       </c>
       <c r="I33" t="inlineStr"/>

</xml_diff>